<commit_message>
tambah contoh di template
</commit_message>
<xml_diff>
--- a/uploads/templates/template_mataKuliah.xlsx
+++ b/uploads/templates/template_mataKuliah.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maranathaedu-my.sharepoint.com/personal/if2072023_student_it_maranatha_edu/Documents/SEMESTER 5/Proyek Perangkat Lunak/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maranathaedu-my.sharepoint.com/personal/if2072023_student_it_maranatha_edu/Documents/SEMESTER 5/Proyek Perangkat Lunak/TubesPPL/uploads/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC104865E91B45CE5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{991C8586-5755-45FA-B15C-83AF0B2EE962}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_F25DC773A252ABDACC104865E91B45CE5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6925976-3DB8-4D9E-9E3B-9FC89BCBBEF5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="2025" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID Mata Kuliah</t>
   </si>
@@ -37,13 +37,31 @@
   </si>
   <si>
     <t>ID Program Studi</t>
+  </si>
+  <si>
+    <t>IN000</t>
+  </si>
+  <si>
+    <t>Contoh Mata Kuliah 1</t>
+  </si>
+  <si>
+    <t>IN001</t>
+  </si>
+  <si>
+    <t>Contoh Mata Kuliah 2</t>
+  </si>
+  <si>
+    <t>IN002</t>
+  </si>
+  <si>
+    <t>Contoh Mata Kuliah 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +73,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,6 +122,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,18 +391,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -391,7 +419,50 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>